<commit_message>
implementação de excluir linhas zeradas e possibilidade de excluir clientes
</commit_message>
<xml_diff>
--- a/devedores.xlsx
+++ b/devedores.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,11 +421,27 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1"/>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Joe</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>R$</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>866.55</t>
+        </is>
+      </c>
+    </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Maria</t>
+          <t>Jose</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -435,14 +451,14 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>-97.55999999999995</t>
+          <t>40</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Joe</t>
+          <t>Arnaldo</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -452,14 +468,14 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>866.55</t>
+          <t>209</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Raimundo</t>
+          <t>Maria</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -469,24 +485,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>390.22</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>R$</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>456</t>
+          <t>450</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
adicionado relatorio detalhado por usuario, relatorio simplificado exibe data do ultimo acerto realizado
</commit_message>
<xml_diff>
--- a/devedores.xlsx
+++ b/devedores.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,113 +421,98 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Joe</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>R$</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>866.55</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>21/12/2020</t>
-        </is>
-      </c>
-    </row>
+    <row r="1"/>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Jose</t>
+          <t>20.0</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>R$</t>
+          <t>Aline</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>110.0</t>
+          <t>22/12/2020</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>21/12/2020</t>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>22/12/2020</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>-30</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>22/12/2020</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>22/12/2020</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>-499</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>22/12/2020</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>22/12/2020</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>20</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Arnaldo</t>
+          <t>500</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>R$</t>
+          <t>Joe</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>219.0</t>
+          <t>22/12/2020</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>21/12/2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Maria</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>R$</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>360.0</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>21/12/2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Moises</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>R$</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>790.0</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>21/12/2020</t>
+          <t>500</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
1 QA test realizado, corrigido as possiveis entradas de formatos invalidos e erros possiveis durante a execução do programa.
</commit_message>
<xml_diff>
--- a/devedores.xlsx
+++ b/devedores.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -425,7 +425,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>20.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -491,6 +491,16 @@
       <c r="N2" t="inlineStr">
         <is>
           <t>20</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>23/12/2020</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>-20</t>
         </is>
       </c>
     </row>
@@ -513,6 +523,128 @@
       <c r="D3" t="inlineStr">
         <is>
           <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>250</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Kiko</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>23/12/2020</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>250</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>220.0</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Ana</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>23/12/2020</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>200</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>23/12/2020</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>70.0</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>23/12/2020</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>70.0</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>23/12/2020</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>70.0</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>23/12/2020</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>70.0</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>23/12/2020</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>70.0</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>23/12/2020</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>70.0</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>23/12/2020</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>70.0</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>23/12/2020</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>-50.0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Inicializando parte 2 do projeto(interface grafica com Tkinter,  implementado na interface: deletar cliente)
</commit_message>
<xml_diff>
--- a/devedores.xlsx
+++ b/devedores.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y5"/>
+  <dimension ref="A1:Z6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -629,22 +629,132 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>550.0</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Kiko</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>23/12/2020</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>250</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Kiko</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>23/12/2020</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>250</t>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>24/12/2020</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>300.0</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>24/12/2020</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>300.0</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>24/12/2020</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>300.0</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>24/12/2020</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>300.0</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>24/12/2020</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>300.0</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>24/12/2020</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>300.0</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>24/12/2020</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>300.0</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>24/12/2020</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>300.0</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>24/12/2020</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>300.0</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>24/12/2020</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>300.0</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>24/12/2020</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>300.0</t>
         </is>
       </c>
     </row>
@@ -746,6 +856,24 @@
         <is>
           <t>-50.0</t>
         </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>500</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Hugo</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>24/12/2020</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
incluido função de cadastro e abatimento de divida.
</commit_message>
<xml_diff>
--- a/devedores.xlsx
+++ b/devedores.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z6"/>
+  <dimension ref="A1:AN17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -629,12 +629,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>550.0</t>
+          <t>220.0</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Kiko</t>
+          <t>Ana</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -642,229 +642,227 @@
           <t>23/12/2020</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>250</t>
-        </is>
+      <c r="D4" t="n">
+        <v>200</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>24/12/2020</t>
+          <t>23/12/2020</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>300.0</t>
+          <t>70.0</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>24/12/2020</t>
+          <t>23/12/2020</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>300.0</t>
+          <t>70.0</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>24/12/2020</t>
+          <t>23/12/2020</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>300.0</t>
+          <t>70.0</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>24/12/2020</t>
+          <t>23/12/2020</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>300.0</t>
+          <t>70.0</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>24/12/2020</t>
+          <t>23/12/2020</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>300.0</t>
+          <t>70.0</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>24/12/2020</t>
+          <t>23/12/2020</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>300.0</t>
+          <t>70.0</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>24/12/2020</t>
+          <t>23/12/2020</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>300.0</t>
+          <t>70.0</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>24/12/2020</t>
+          <t>23/12/2020</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>300.0</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>24/12/2020</t>
-        </is>
-      </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>300.0</t>
-        </is>
-      </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>24/12/2020</t>
-        </is>
-      </c>
-      <c r="X4" t="inlineStr">
-        <is>
-          <t>300.0</t>
-        </is>
-      </c>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>24/12/2020</t>
-        </is>
-      </c>
-      <c r="Z4" t="inlineStr">
-        <is>
-          <t>300.0</t>
+          <t>-50.0</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>220.0</t>
+          <t>589.0</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Ana</t>
+          <t>Hugo</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>23/12/2020</t>
+          <t>24/12/2020</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>23/12/2020</t>
+          <t>25/12/2020</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>70.0</t>
+          <t>89.0</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>23/12/2020</t>
+          <t>25/12/2020</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>70.0</t>
+          <t>89.0</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>23/12/2020</t>
+          <t>25/12/2020</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>70.0</t>
+          <t>89.0</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>23/12/2020</t>
+          <t>25/12/2020</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>70.0</t>
+          <t>89.0</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>23/12/2020</t>
+          <t>25/12/2020</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>70.0</t>
+          <t>89.0</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>23/12/2020</t>
+          <t>25/12/2020</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>70.0</t>
+          <t>89.0</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>23/12/2020</t>
+          <t>25/12/2020</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>70.0</t>
+          <t>89.0</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>23/12/2020</t>
+          <t>25/12/2020</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>-50.0</t>
+          <t>89.0</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>89.0</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>89.0</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>89.0</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Hugo</t>
+          <t>Moises</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -873,7 +871,509 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>500</v>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>350</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Joaquim</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>24/12/2020</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>300</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Kirliaa</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>24/12/2020</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>880.0</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Juka</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>24/12/2020</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>800</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>80.0</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>80.0</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>80.0</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>80.0</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>80.0</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>80.0</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>80.0</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>80.0</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>80.0</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>80.0</t>
+        </is>
+      </c>
+      <c r="Y9" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="Z9" t="inlineStr">
+        <is>
+          <t>80.0</t>
+        </is>
+      </c>
+      <c r="AA9" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="AB9" t="inlineStr">
+        <is>
+          <t>80.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>900</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Oseias</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>24/12/2020</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>890</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Haas</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>24/12/2020</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>900</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Test2</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>24/12/2020</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>670</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Janete</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>24/12/2020</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>700</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Cleide</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>24/12/2020</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>670</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>June</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>24/12/2020</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>789.65</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Jurema</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>789.65</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>85.0</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Joarez</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>976</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>-267.0</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>-267.0</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>-267.0</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>-267.0</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>-267.0</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>-267.0</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>-267.0</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>-267.0</t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="V17" t="inlineStr">
+        <is>
+          <t>-267.0</t>
+        </is>
+      </c>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="X17" t="inlineStr">
+        <is>
+          <t>-267.0</t>
+        </is>
+      </c>
+      <c r="Y17" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="Z17" t="inlineStr">
+        <is>
+          <t>-267.0</t>
+        </is>
+      </c>
+      <c r="AA17" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="AB17" t="inlineStr">
+        <is>
+          <t>-267.0</t>
+        </is>
+      </c>
+      <c r="AC17" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="AD17" t="inlineStr">
+        <is>
+          <t>-267.0</t>
+        </is>
+      </c>
+      <c r="AE17" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="AF17" t="inlineStr">
+        <is>
+          <t>50.0</t>
+        </is>
+      </c>
+      <c r="AG17" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="AH17" t="inlineStr">
+        <is>
+          <t>-560.0</t>
+        </is>
+      </c>
+      <c r="AI17" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="AJ17" t="inlineStr">
+        <is>
+          <t>-20.0</t>
+        </is>
+      </c>
+      <c r="AK17" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="AL17" t="inlineStr">
+        <is>
+          <t>-10.0</t>
+        </is>
+      </c>
+      <c r="AM17" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="AN17" t="inlineStr">
+        <is>
+          <t>-5.0</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implementação de relatorio simples
</commit_message>
<xml_diff>
--- a/devedores.xlsx
+++ b/devedores.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AN17"/>
+  <dimension ref="A1:CD20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1100.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -623,6 +623,266 @@
       <c r="X3" t="inlineStr">
         <is>
           <t>600.0</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>-50.0</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>-50.0</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>-50.0</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>-50.0</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t>-50.0</t>
+        </is>
+      </c>
+      <c r="AI3" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="AJ3" t="inlineStr">
+        <is>
+          <t>-50.0</t>
+        </is>
+      </c>
+      <c r="AK3" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="AL3" t="inlineStr">
+        <is>
+          <t>-50.0</t>
+        </is>
+      </c>
+      <c r="AM3" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="AN3" t="inlineStr">
+        <is>
+          <t>-50.0</t>
+        </is>
+      </c>
+      <c r="AO3" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="AP3" t="inlineStr">
+        <is>
+          <t>-50.0</t>
+        </is>
+      </c>
+      <c r="AQ3" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="AR3" t="inlineStr">
+        <is>
+          <t>-50.0</t>
+        </is>
+      </c>
+      <c r="AS3" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="AT3" t="inlineStr">
+        <is>
+          <t>-50.0</t>
+        </is>
+      </c>
+      <c r="AU3" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="AV3" t="inlineStr">
+        <is>
+          <t>-50.0</t>
+        </is>
+      </c>
+      <c r="AW3" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="AX3" t="inlineStr">
+        <is>
+          <t>-50.0</t>
+        </is>
+      </c>
+      <c r="AY3" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="AZ3" t="inlineStr">
+        <is>
+          <t>-50.0</t>
+        </is>
+      </c>
+      <c r="BA3" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BB3" t="inlineStr">
+        <is>
+          <t>-50.0</t>
+        </is>
+      </c>
+      <c r="BC3" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BD3" t="inlineStr">
+        <is>
+          <t>-50.0</t>
+        </is>
+      </c>
+      <c r="BE3" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BF3" t="inlineStr">
+        <is>
+          <t>-50.0</t>
+        </is>
+      </c>
+      <c r="BG3" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BH3" t="inlineStr">
+        <is>
+          <t>-50.0</t>
+        </is>
+      </c>
+      <c r="BI3" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BJ3" t="inlineStr">
+        <is>
+          <t>-50.0</t>
+        </is>
+      </c>
+      <c r="BK3" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BL3" t="inlineStr">
+        <is>
+          <t>-50.0</t>
+        </is>
+      </c>
+      <c r="BM3" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BN3" t="inlineStr">
+        <is>
+          <t>-50.0</t>
+        </is>
+      </c>
+      <c r="BO3" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BP3" t="inlineStr">
+        <is>
+          <t>-50.0</t>
+        </is>
+      </c>
+      <c r="BQ3" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BR3" t="inlineStr">
+        <is>
+          <t>-50.0</t>
+        </is>
+      </c>
+      <c r="BS3" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BT3" t="inlineStr">
+        <is>
+          <t>-50.0</t>
+        </is>
+      </c>
+      <c r="BU3" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BV3" t="inlineStr">
+        <is>
+          <t>-50.0</t>
+        </is>
+      </c>
+      <c r="BW3" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BX3" t="inlineStr">
+        <is>
+          <t>-1050.0</t>
         </is>
       </c>
     </row>
@@ -729,7 +989,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>589.0</t>
+          <t>600.0</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -853,6 +1113,196 @@
       <c r="Z5" t="inlineStr">
         <is>
           <t>89.0</t>
+        </is>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t>70.0</t>
+        </is>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t>70.0</t>
+        </is>
+      </c>
+      <c r="AE5" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="AF5" t="inlineStr">
+        <is>
+          <t>70.0</t>
+        </is>
+      </c>
+      <c r="AG5" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="AH5" t="inlineStr">
+        <is>
+          <t>70.0</t>
+        </is>
+      </c>
+      <c r="AI5" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="AJ5" t="inlineStr">
+        <is>
+          <t>70.0</t>
+        </is>
+      </c>
+      <c r="AK5" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="AL5" t="inlineStr">
+        <is>
+          <t>70.0</t>
+        </is>
+      </c>
+      <c r="AM5" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="AN5" t="inlineStr">
+        <is>
+          <t>70.0</t>
+        </is>
+      </c>
+      <c r="AO5" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="AP5" t="inlineStr">
+        <is>
+          <t>70.0</t>
+        </is>
+      </c>
+      <c r="AQ5" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="AR5" t="inlineStr">
+        <is>
+          <t>70.0</t>
+        </is>
+      </c>
+      <c r="AS5" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="AT5" t="inlineStr">
+        <is>
+          <t>70.0</t>
+        </is>
+      </c>
+      <c r="AU5" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="AV5" t="inlineStr">
+        <is>
+          <t>70.0</t>
+        </is>
+      </c>
+      <c r="AW5" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="AX5" t="inlineStr">
+        <is>
+          <t>70.0</t>
+        </is>
+      </c>
+      <c r="AY5" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="AZ5" t="inlineStr">
+        <is>
+          <t>70.0</t>
+        </is>
+      </c>
+      <c r="BA5" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="BB5" t="inlineStr">
+        <is>
+          <t>70.0</t>
+        </is>
+      </c>
+      <c r="BC5" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="BD5" t="inlineStr">
+        <is>
+          <t>70.0</t>
+        </is>
+      </c>
+      <c r="BE5" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="BF5" t="inlineStr">
+        <is>
+          <t>70.0</t>
+        </is>
+      </c>
+      <c r="BG5" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="BH5" t="inlineStr">
+        <is>
+          <t>70.0</t>
+        </is>
+      </c>
+      <c r="BI5" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="BJ5" t="inlineStr">
+        <is>
+          <t>70.0</t>
+        </is>
+      </c>
+      <c r="BK5" t="inlineStr">
+        <is>
+          <t>25/12/2020</t>
+        </is>
+      </c>
+      <c r="BL5" t="inlineStr">
+        <is>
+          <t>-59.0</t>
         </is>
       </c>
     </row>
@@ -1124,11 +1574,11 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>700</v>
+        <v>670</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Cleide</t>
+          <t>June</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1137,227 +1587,599 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>700</v>
+        <v>670</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>670</v>
+        <v>789.65</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>June</t>
+          <t>Jurema</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>24/12/2020</t>
+          <t>25/12/2020</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>670</v>
+        <v>789.65</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
-        <v>789.65</v>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>20.0</t>
+        </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Jurema</t>
+          <t>Teste</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>25/12/2020</t>
+          <t>26/12/2020</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>789.65</v>
+        <v>10</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="V16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="X16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="Y16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="Z16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="AA16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="AB16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="AC16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="AD16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="AE16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="AF16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="AG16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="AH16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="AI16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="AJ16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="AK16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="AL16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="AM16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="AN16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="AO16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="AP16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="AQ16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="AR16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="AS16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="AT16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="AU16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="AV16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="AW16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="AX16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="AY16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="AZ16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="BA16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BB16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="BC16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BD16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="BE16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BF16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="BG16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BH16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="BI16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BJ16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="BK16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BL16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="BM16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BN16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="BO16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BP16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="BQ16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BR16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="BS16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BT16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="BU16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BV16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="BW16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BX16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="BY16" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BZ16" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>85.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Joarez</t>
+          <t>Aba</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>25/12/2020</t>
+          <t>26/12/2020</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>976</v>
+        <v>10</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>25/12/2020</t>
+          <t>26/12/2020</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>-267.0</t>
+          <t>-10.0</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>25/12/2020</t>
+          <t>26/12/2020</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>-267.0</t>
+          <t>-10.0</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>25/12/2020</t>
+          <t>26/12/2020</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>-267.0</t>
+          <t>-10.0</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>25/12/2020</t>
+          <t>26/12/2020</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>-267.0</t>
+          <t>-10.0</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>25/12/2020</t>
+          <t>26/12/2020</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>-267.0</t>
+          <t>-10.0</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>25/12/2020</t>
+          <t>26/12/2020</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>-267.0</t>
+          <t>-10.0</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>25/12/2020</t>
+          <t>26/12/2020</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
         <is>
-          <t>-267.0</t>
+          <t>-10.0</t>
         </is>
       </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>25/12/2020</t>
+          <t>26/12/2020</t>
         </is>
       </c>
       <c r="T17" t="inlineStr">
         <is>
-          <t>-267.0</t>
+          <t>-10.0</t>
         </is>
       </c>
       <c r="U17" t="inlineStr">
         <is>
-          <t>25/12/2020</t>
+          <t>26/12/2020</t>
         </is>
       </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>-267.0</t>
+          <t>-10.0</t>
         </is>
       </c>
       <c r="W17" t="inlineStr">
         <is>
-          <t>25/12/2020</t>
+          <t>26/12/2020</t>
         </is>
       </c>
       <c r="X17" t="inlineStr">
         <is>
-          <t>-267.0</t>
+          <t>-10.0</t>
         </is>
       </c>
       <c r="Y17" t="inlineStr">
         <is>
-          <t>25/12/2020</t>
+          <t>26/12/2020</t>
         </is>
       </c>
       <c r="Z17" t="inlineStr">
         <is>
-          <t>-267.0</t>
+          <t>-10.0</t>
         </is>
       </c>
       <c r="AA17" t="inlineStr">
         <is>
-          <t>25/12/2020</t>
+          <t>26/12/2020</t>
         </is>
       </c>
       <c r="AB17" t="inlineStr">
         <is>
-          <t>-267.0</t>
+          <t>-10.0</t>
         </is>
       </c>
       <c r="AC17" t="inlineStr">
         <is>
-          <t>25/12/2020</t>
+          <t>26/12/2020</t>
         </is>
       </c>
       <c r="AD17" t="inlineStr">
         <is>
-          <t>-267.0</t>
+          <t>-10.0</t>
         </is>
       </c>
       <c r="AE17" t="inlineStr">
         <is>
-          <t>25/12/2020</t>
+          <t>26/12/2020</t>
         </is>
       </c>
       <c r="AF17" t="inlineStr">
         <is>
-          <t>50.0</t>
+          <t>-10.0</t>
         </is>
       </c>
       <c r="AG17" t="inlineStr">
         <is>
-          <t>25/12/2020</t>
+          <t>26/12/2020</t>
         </is>
       </c>
       <c r="AH17" t="inlineStr">
         <is>
-          <t>-560.0</t>
+          <t>-10.0</t>
         </is>
       </c>
       <c r="AI17" t="inlineStr">
         <is>
-          <t>25/12/2020</t>
+          <t>26/12/2020</t>
         </is>
       </c>
       <c r="AJ17" t="inlineStr">
         <is>
-          <t>-20.0</t>
+          <t>-10.0</t>
         </is>
       </c>
       <c r="AK17" t="inlineStr">
         <is>
-          <t>25/12/2020</t>
+          <t>26/12/2020</t>
         </is>
       </c>
       <c r="AL17" t="inlineStr">
@@ -1367,12 +2189,300 @@
       </c>
       <c r="AM17" t="inlineStr">
         <is>
-          <t>25/12/2020</t>
+          <t>26/12/2020</t>
         </is>
       </c>
       <c r="AN17" t="inlineStr">
         <is>
-          <t>-5.0</t>
+          <t>-10.0</t>
+        </is>
+      </c>
+      <c r="AO17" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="AP17" t="inlineStr">
+        <is>
+          <t>-10.0</t>
+        </is>
+      </c>
+      <c r="AQ17" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="AR17" t="inlineStr">
+        <is>
+          <t>-10.0</t>
+        </is>
+      </c>
+      <c r="AS17" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="AT17" t="inlineStr">
+        <is>
+          <t>-10.0</t>
+        </is>
+      </c>
+      <c r="AU17" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="AV17" t="inlineStr">
+        <is>
+          <t>-10.0</t>
+        </is>
+      </c>
+      <c r="AW17" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="AX17" t="inlineStr">
+        <is>
+          <t>-10.0</t>
+        </is>
+      </c>
+      <c r="AY17" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="AZ17" t="inlineStr">
+        <is>
+          <t>-10.0</t>
+        </is>
+      </c>
+      <c r="BA17" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BB17" t="inlineStr">
+        <is>
+          <t>-10.0</t>
+        </is>
+      </c>
+      <c r="BC17" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BD17" t="inlineStr">
+        <is>
+          <t>-10.0</t>
+        </is>
+      </c>
+      <c r="BE17" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BF17" t="inlineStr">
+        <is>
+          <t>-10.0</t>
+        </is>
+      </c>
+      <c r="BG17" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BH17" t="inlineStr">
+        <is>
+          <t>-10.0</t>
+        </is>
+      </c>
+      <c r="BI17" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BJ17" t="inlineStr">
+        <is>
+          <t>-10.0</t>
+        </is>
+      </c>
+      <c r="BK17" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BL17" t="inlineStr">
+        <is>
+          <t>-10.0</t>
+        </is>
+      </c>
+      <c r="BM17" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BN17" t="inlineStr">
+        <is>
+          <t>-10.0</t>
+        </is>
+      </c>
+      <c r="BO17" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BP17" t="inlineStr">
+        <is>
+          <t>-10.0</t>
+        </is>
+      </c>
+      <c r="BQ17" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BR17" t="inlineStr">
+        <is>
+          <t>-10.0</t>
+        </is>
+      </c>
+      <c r="BS17" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BT17" t="inlineStr">
+        <is>
+          <t>-10.0</t>
+        </is>
+      </c>
+      <c r="BU17" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BV17" t="inlineStr">
+        <is>
+          <t>-10.0</t>
+        </is>
+      </c>
+      <c r="BW17" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BX17" t="inlineStr">
+        <is>
+          <t>-10.0</t>
+        </is>
+      </c>
+      <c r="BY17" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="BZ17" t="inlineStr">
+        <is>
+          <t>-10.0</t>
+        </is>
+      </c>
+      <c r="CA17" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="CB17" t="inlineStr">
+        <is>
+          <t>-10.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>100</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Taki</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>80.0</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Jack</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>60</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>20.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Teste12</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>10</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>26/12/2020</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>-10.0</t>
         </is>
       </c>
     </row>

</xml_diff>